<commit_message>
Màj Word avec coorrection
</commit_message>
<xml_diff>
--- a/Calcul écarts test.xlsx
+++ b/Calcul écarts test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\Cours 3ème année\PJE\GitHub\geometry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{654E7D4F-D381-44F6-8CAE-37B9542F9558}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B03E5BA9-CE89-4A07-8AAF-A499B6E173AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="380" windowWidth="14400" windowHeight="7810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -103,7 +103,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -142,36 +142,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
@@ -339,46 +309,44 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -663,65 +631,65 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.81640625" style="16" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" style="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="14" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="10"/>
-      <c r="B1" s="17"/>
-      <c r="C1" s="18" t="s">
+    <row r="1" spans="1:8" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="8"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="H1" s="14" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="6">
         <v>1010</v>
       </c>
-      <c r="D2" s="8">
+      <c r="D2" s="6">
         <v>1320</v>
       </c>
-      <c r="E2" s="8">
+      <c r="E2" s="6">
         <v>1010</v>
       </c>
-      <c r="F2" s="8">
+      <c r="F2" s="6">
         <v>1320</v>
       </c>
-      <c r="G2" s="8">
+      <c r="G2" s="6">
         <v>1010</v>
       </c>
-      <c r="H2" s="9">
+      <c r="H2" s="7">
         <v>1075</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="12"/>
-      <c r="B3" s="5" t="s">
+      <c r="A3" s="16"/>
+      <c r="B3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="1">
@@ -744,10 +712,10 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="1">
@@ -770,8 +738,8 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="12"/>
-      <c r="B5" s="5" t="s">
+      <c r="A5" s="16"/>
+      <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="1">
@@ -794,8 +762,8 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="15"/>
-      <c r="B6" s="5"/>
+      <c r="A6" s="9"/>
+      <c r="B6" s="3"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -804,10 +772,10 @@
       <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="1">
@@ -836,8 +804,8 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="12"/>
-      <c r="B8" s="5" t="s">
+      <c r="A8" s="16"/>
+      <c r="B8" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="1">
@@ -866,8 +834,8 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="15"/>
-      <c r="B9" s="5"/>
+      <c r="A9" s="9"/>
+      <c r="B9" s="3"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -876,63 +844,63 @@
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="1">
-        <f>C2-C4</f>
+        <f>ABS(C2-C4)</f>
         <v>53.848861319508728</v>
       </c>
       <c r="D10" s="1">
-        <f t="shared" ref="D10:H11" si="1">D2-D4</f>
+        <f t="shared" ref="D10:H11" si="1">ABS(D2-D4)</f>
         <v>62.731134561902991</v>
       </c>
       <c r="E10" s="1">
         <f t="shared" si="1"/>
-        <v>-45.758021518189025</v>
+        <v>45.758021518189025</v>
       </c>
       <c r="F10" s="1">
         <f t="shared" si="1"/>
-        <v>-14.587951391740035</v>
+        <v>14.587951391740035</v>
       </c>
       <c r="G10" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H10" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="13"/>
-      <c r="B11" s="6" t="s">
+      <c r="A11" s="17"/>
+      <c r="B11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="3">
-        <f>C3-C5</f>
+      <c r="C11" s="1">
+        <f>ABS(C3-C5)</f>
         <v>49.682634537263993</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="1">
         <f t="shared" si="1"/>
-        <v>-14.663637119793293</v>
-      </c>
-      <c r="E11" s="3">
+        <v>14.663637119793293</v>
+      </c>
+      <c r="E11" s="1">
         <f t="shared" si="1"/>
         <v>43.035482870094029</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="1">
         <f t="shared" si="1"/>
         <v>14.179162758702887</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G11" s="1">
         <f t="shared" si="1"/>
         <v>75.028824506888895</v>
       </c>
-      <c r="H11" s="4">
+      <c r="H11" s="1">
         <f t="shared" si="1"/>
         <v>75.028824506890942</v>
       </c>

</xml_diff>